<commit_message>
add a few attributues to SplashBrowser to support crawling
</commit_message>
<xml_diff>
--- a/tests/books_toscrape/book_titles.xlsx
+++ b/tests/books_toscrape/book_titles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjord\repos\transistor\tests\books_toscrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3365AF68-79D6-4926-8B6A-287D932BFD1A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B86EFB-B2DD-453C-8B37-19FBCFFDF6AA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11685" windowHeight="4148" xr2:uid="{A981794D-1504-4842-AF12-31D3D191C2DD}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>